<commit_message>
Update file specification based on findings from the initial data drop from all partners.
</commit_message>
<xml_diff>
--- a/InTrust-FileFormatSpecification.xlsx
+++ b/InTrust-FileFormatSpecification.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="V:\Dropbox\BlueSun\APEXA\General\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="V:\Drive\BlueSun\APEXA\System Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -17,12 +17,10 @@
     <sheet name="Company" sheetId="3" r:id="rId3"/>
     <sheet name="Address" sheetId="6" r:id="rId4"/>
     <sheet name="Phone" sheetId="7" r:id="rId5"/>
-    <sheet name="Shareholder" sheetId="9" r:id="rId6"/>
-    <sheet name="Contract" sheetId="11" r:id="rId7"/>
-    <sheet name="Rate" sheetId="15" r:id="rId8"/>
-    <sheet name="Merged Broker Code" sheetId="14" r:id="rId9"/>
-    <sheet name="License" sheetId="12" r:id="rId10"/>
-    <sheet name="E&amp;O" sheetId="16" r:id="rId11"/>
+    <sheet name="Contract" sheetId="11" r:id="rId6"/>
+    <sheet name="Merged Broker Code" sheetId="14" r:id="rId7"/>
+    <sheet name="License" sheetId="12" r:id="rId8"/>
+    <sheet name="E&amp;O" sheetId="16" r:id="rId9"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -34,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="110">
   <si>
     <t>Number</t>
   </si>
@@ -105,12 +103,6 @@
     <t>Date of Birth</t>
   </si>
   <si>
-    <t>Social Insurance Number</t>
-  </si>
-  <si>
-    <t>Driver's License Number</t>
-  </si>
-  <si>
     <t>Male / Female</t>
   </si>
   <si>
@@ -138,12 +130,6 @@
     <t>YYYY-MM-DD</t>
   </si>
   <si>
-    <t>999-999-999</t>
-  </si>
-  <si>
-    <t>A9999-99999-99999</t>
-  </si>
-  <si>
     <t>Text</t>
   </si>
   <si>
@@ -222,24 +208,12 @@
     <t>Contact Person's Name</t>
   </si>
   <si>
-    <t>The ID linking this record to the related company record.</t>
-  </si>
-  <si>
-    <t>Percentage</t>
-  </si>
-  <si>
     <t>Phone Number</t>
   </si>
   <si>
     <t>The phone extension if one is required.</t>
   </si>
   <si>
-    <t>Linked AdvisorId</t>
-  </si>
-  <si>
-    <t>The ID linking to an advisor record if the shareholder is also an advisor.</t>
-  </si>
-  <si>
     <t>ContractId</t>
   </si>
   <si>
@@ -288,21 +262,12 @@
     <t>The ID linking to the associated contract.</t>
   </si>
   <si>
-    <t>Line of Business</t>
-  </si>
-  <si>
-    <t>Rate</t>
-  </si>
-  <si>
     <t>Source</t>
   </si>
   <si>
     <t>Information identifying the source of this code before it was merged.</t>
   </si>
   <si>
-    <t>Master Contract Number</t>
-  </si>
-  <si>
     <t>Provider</t>
   </si>
   <si>
@@ -312,27 +277,6 @@
     <t>Crow's Foot Notation</t>
   </si>
   <si>
-    <t>This Excel file should provide details regarding the fields required for the data extract.  The format that this data is delivered in can either be a set of flat CSV files, an XML structure, or a SQL Server backup file.  Each tab of this spreadsheet should describe the data expected in each file, section, or table and the diagram below has been provided to help navigate the relationships between the data in the tabs.  The diagram below uses standard crow's foot notation (see diagram on the right for assistance).</t>
-  </si>
-  <si>
-    <t>Last Payment Date</t>
-  </si>
-  <si>
-    <t>The last payment made to the advisor based on this contract.</t>
-  </si>
-  <si>
-    <t>Last Payment Cents</t>
-  </si>
-  <si>
-    <t>The cent value of the last payment (e.g. 123.45 would be 45).</t>
-  </si>
-  <si>
-    <t>The last 4 digits of the bank account that corresponds to the last payment information provided above.</t>
-  </si>
-  <si>
-    <t>Bank Account (Last 4 Digits)</t>
-  </si>
-  <si>
     <t>Name of the MGA this contract was through.</t>
   </si>
   <si>
@@ -354,18 +298,9 @@
     <t>Need for attestation, would like to use for deduplication.</t>
   </si>
   <si>
-    <t>Percentage of the company owned.</t>
-  </si>
-  <si>
     <t>Providing as many additional broker codes as possible will help match this contract with additional MGA records.</t>
   </si>
   <si>
-    <t>Sub-Contract Number</t>
-  </si>
-  <si>
-    <t>Need for attestation, but would like to use for deduplication.</t>
-  </si>
-  <si>
     <t>Province</t>
   </si>
   <si>
@@ -376,6 +311,57 @@
   </si>
   <si>
     <t>This will help you push different documents to advisors with different historical contracts.</t>
+  </si>
+  <si>
+    <t>If not provided, we default based on primary language of Province.</t>
+  </si>
+  <si>
+    <t>If not provided, we default to Home.</t>
+  </si>
+  <si>
+    <t>Carrier Name</t>
+  </si>
+  <si>
+    <t>Carrier Code</t>
+  </si>
+  <si>
+    <t>Name of the Carrier this contract was through.</t>
+  </si>
+  <si>
+    <t>An ID representing the Carrier if one exists.</t>
+  </si>
+  <si>
+    <t>Contract Date</t>
+  </si>
+  <si>
+    <t>Date the contract was established.</t>
+  </si>
+  <si>
+    <t>If not provided, we default to Active.</t>
+  </si>
+  <si>
+    <t>Termination Date</t>
+  </si>
+  <si>
+    <t>Date the contract was terminated.</t>
+  </si>
+  <si>
+    <t>CIPR Number</t>
+  </si>
+  <si>
+    <t>Unique ID assigned by Alberta.</t>
+  </si>
+  <si>
+    <t>Start Date</t>
+  </si>
+  <si>
+    <t>Policy Number</t>
+  </si>
+  <si>
+    <t>Certificate Number</t>
+  </si>
+  <si>
+    <t>This Excel file should provide details regarding the fields required for the data extract.  The format that this data is delivered in can either be a set of flat CSV files.  Each tab of this spreadsheet should describe the data expected in each file, section, or table and the diagram below has been provided to help navigate the relationships between the data in the tabs.  The diagram below uses standard crow's foot notation (see diagram on the right for assistance).</t>
   </si>
 </sst>
 </file>
@@ -436,12 +422,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -450,6 +430,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -528,15 +514,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
+      <xdr:colOff>1</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>133269</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>117716</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -553,8 +539,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="628650" y="1152525"/>
-          <a:ext cx="7277100" cy="6219744"/>
+          <a:off x="609601" y="1143000"/>
+          <a:ext cx="7315200" cy="6404216"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -829,6 +815,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="B2:W6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -839,88 +826,88 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="S2" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="T2" s="7"/>
-      <c r="U2" s="7"/>
-      <c r="V2" s="7"/>
-      <c r="W2" s="7"/>
+      <c r="B2" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+      <c r="S2" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="T2" s="10"/>
+      <c r="U2" s="10"/>
+      <c r="V2" s="10"/>
+      <c r="W2" s="10"/>
     </row>
     <row r="3" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="S3" s="7"/>
-      <c r="T3" s="7"/>
-      <c r="U3" s="7"/>
-      <c r="V3" s="7"/>
-      <c r="W3" s="7"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+      <c r="S3" s="10"/>
+      <c r="T3" s="10"/>
+      <c r="U3" s="10"/>
+      <c r="V3" s="10"/>
+      <c r="W3" s="10"/>
     </row>
     <row r="4" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
     </row>
     <row r="5" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
     </row>
     <row r="6" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="6"/>
-      <c r="M6" s="6"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -933,9 +920,10 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E11"/>
+  <sheetPr codeName="Sheet2"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -953,7 +941,7 @@
         <v>9</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>6</v>
@@ -965,9 +953,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>50</v>
+        <v>14</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>12</v>
@@ -976,40 +964,34 @@
         <v>13</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>51</v>
+        <v>16</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>53</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B4" s="3">
-        <v>99999999</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>13</v>
+        <v>18</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>72</v>
+        <v>5</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>13</v>
@@ -1017,60 +999,95 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>74</v>
+        <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>57</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>76</v>
+        <v>3</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>73</v>
+        <v>19</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>75</v>
+        <v>20</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>110</v>
+        <v>21</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>13</v>
       </c>
+      <c r="E11" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="7"/>
+      <c r="D14" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="E14" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1078,8 +1095,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1098,7 +1116,7 @@
         <v>9</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>6</v>
@@ -1110,9 +1128,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>12</v>
@@ -1121,77 +1139,73 @@
         <v>13</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>51</v>
+        <v>26</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>53</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>88</v>
+        <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="B5" s="3">
+        <v>999999999</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>13</v>
+        <v>30</v>
+      </c>
+      <c r="B6" s="3">
+        <v>9999999999</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>7</v>
+        <v>57</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>13</v>
-      </c>
+      <c r="A8" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="7"/>
+      <c r="D8" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="E8" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1199,9 +1213,10 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E15"/>
+  <sheetPr codeName="Sheet4"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1219,7 +1234,7 @@
         <v>9</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>6</v>
@@ -1231,9 +1246,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>46</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>12</v>
@@ -1242,34 +1257,46 @@
         <v>13</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>16</v>
+        <v>47</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>12</v>
+        <v>48</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>13</v>
@@ -1277,18 +1304,18 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>4</v>
+        <v>36</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>3</v>
+        <v>37</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>13</v>
@@ -1296,75 +1323,38 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>1</v>
+        <v>41</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>25</v>
+        <v>43</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1373,8 +1363,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1393,7 +1384,7 @@
         <v>9</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>6</v>
@@ -1405,9 +1396,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>12</v>
@@ -1416,59 +1407,71 @@
         <v>13</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>12</v>
+        <v>48</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>13</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B5" s="3">
-        <v>999999999</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B6" s="3">
-        <v>9999999999</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>105</v>
+        <v>58</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>36</v>
+        <v>56</v>
+      </c>
+      <c r="B7" s="3">
+        <v>999999</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1477,9 +1480,10 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E10"/>
+  <sheetPr codeName="Sheet6"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1497,7 +1501,7 @@
         <v>9</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>6</v>
@@ -1509,9 +1513,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>12</v>
@@ -1520,29 +1524,29 @@
         <v>13</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>52</v>
+        <v>12</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>13</v>
@@ -1551,70 +1555,169 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>13</v>
+    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="D5" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>36</v>
-      </c>
+      <c r="A6" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="E6" s="8"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>13</v>
-      </c>
+      <c r="A7" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="E7" s="8"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>44</v>
+        <v>73</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>43</v>
+        <v>32</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>45</v>
+        <v>70</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>47</v>
+        <v>12</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>48</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>42</v>
+        <v>71</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -1623,9 +1726,10 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <sheetPr codeName="Sheet7"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1643,7 +1747,7 @@
         <v>9</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>6</v>
@@ -1655,9 +1759,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>12</v>
@@ -1666,68 +1770,32 @@
         <v>13</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>51</v>
+        <v>69</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>52</v>
+        <v>12</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>53</v>
+      <c r="E3" s="2" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>38</v>
+        <v>76</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B7" s="3">
-        <v>999999</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -1736,8 +1804,163 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet8"/>
+  <dimension ref="A1:E12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="11" style="3" customWidth="1"/>
+    <col min="4" max="4" width="44.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="32.5703125" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" s="3">
+        <v>99999999</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="7"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1756,7 +1979,7 @@
         <v>9</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>6</v>
@@ -1770,447 +1993,70 @@
     </row>
     <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>13</v>
-      </c>
       <c r="D2" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>36</v>
+        <v>48</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>13</v>
-      </c>
+      <c r="A4" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>36</v>
-      </c>
+      <c r="A5" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>3</v>
+        <v>78</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>63</v>
+        <v>7</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="28.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="21.42578125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="11" style="3" customWidth="1"/>
-    <col min="4" max="4" width="44.7109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="32.5703125" style="2" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="9"/>
-      <c r="D5" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>100</v>
-      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>79</v>
+        <v>8</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="28.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="21.42578125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="11" style="3" customWidth="1"/>
-    <col min="4" max="4" width="44.7109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="32.5703125" style="2" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="28.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="21.42578125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="11" style="3" customWidth="1"/>
-    <col min="4" max="4" width="44.7109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="32.5703125" style="2" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>87</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add email to company record.
</commit_message>
<xml_diff>
--- a/InTrust-FileFormatSpecification.xlsx
+++ b/InTrust-FileFormatSpecification.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="V:\Drive\BlueSun\APEXA\System Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="V:\GIT_2015\intrust-file-specification\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="110">
   <si>
     <t>Number</t>
   </si>
@@ -1098,7 +1098,7 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1188,24 +1188,35 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+      <c r="B8" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="B8" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="8" t="s">
+      <c r="B9" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="7"/>
+      <c r="D9" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="E8" s="8"/>
+      <c r="E9" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update specification to support the full hierarchy of contracts.
</commit_message>
<xml_diff>
--- a/InTrust-FileFormatSpecification.xlsx
+++ b/InTrust-FileFormatSpecification.xlsx
@@ -2,37 +2,33 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="V:\GIT_2015\intrust-file-specification\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="V:\Drive\BlueSun\APEXA\System Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="28800" windowHeight="12420"/>
   </bookViews>
   <sheets>
-    <sheet name="Data Diagram" sheetId="8" r:id="rId1"/>
-    <sheet name="Advisor" sheetId="2" r:id="rId2"/>
-    <sheet name="Company" sheetId="3" r:id="rId3"/>
-    <sheet name="Address" sheetId="6" r:id="rId4"/>
-    <sheet name="Phone" sheetId="7" r:id="rId5"/>
-    <sheet name="Contract" sheetId="11" r:id="rId6"/>
-    <sheet name="Merged Broker Code" sheetId="14" r:id="rId7"/>
-    <sheet name="License" sheetId="12" r:id="rId8"/>
-    <sheet name="E&amp;O" sheetId="16" r:id="rId9"/>
+    <sheet name="Changes-Jan2016" sheetId="17" r:id="rId1"/>
+    <sheet name="Data Diagram" sheetId="8" r:id="rId2"/>
+    <sheet name="Advisor" sheetId="2" r:id="rId3"/>
+    <sheet name="Company" sheetId="3" r:id="rId4"/>
+    <sheet name="Address" sheetId="6" r:id="rId5"/>
+    <sheet name="Phone" sheetId="7" r:id="rId6"/>
+    <sheet name="Contract" sheetId="11" r:id="rId7"/>
+    <sheet name="Merged Broker Code" sheetId="14" r:id="rId8"/>
+    <sheet name="License" sheetId="12" r:id="rId9"/>
+    <sheet name="E&amp;O" sheetId="16" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="123">
   <si>
     <t>Number</t>
   </si>
@@ -244,21 +240,6 @@
     <t>Broker Code</t>
   </si>
   <si>
-    <t>MGA Code</t>
-  </si>
-  <si>
-    <t>MGA Branch Code</t>
-  </si>
-  <si>
-    <t>AGA Code</t>
-  </si>
-  <si>
-    <t>MGA Name</t>
-  </si>
-  <si>
-    <t>AGA Name</t>
-  </si>
-  <si>
     <t>The ID linking to the associated contract.</t>
   </si>
   <si>
@@ -277,21 +258,6 @@
     <t>Crow's Foot Notation</t>
   </si>
   <si>
-    <t>Name of the MGA this contract was through.</t>
-  </si>
-  <si>
-    <t>An ID representing the MGA if one exists.</t>
-  </si>
-  <si>
-    <t>An ID for a subdivision of the MGA if one exists.</t>
-  </si>
-  <si>
-    <t>The name of the AGA this contract was through if one exists.</t>
-  </si>
-  <si>
-    <t>An ID representing the AGA if one exists.</t>
-  </si>
-  <si>
     <t>The unique ID assigned to the advisor once all of the contracts have been signed.  Sometimes also referred to as Carrier Code, Contract Code, or Selling Code.</t>
   </si>
   <si>
@@ -319,18 +285,6 @@
     <t>If not provided, we default to Home.</t>
   </si>
   <si>
-    <t>Carrier Name</t>
-  </si>
-  <si>
-    <t>Carrier Code</t>
-  </si>
-  <si>
-    <t>Name of the Carrier this contract was through.</t>
-  </si>
-  <si>
-    <t>An ID representing the Carrier if one exists.</t>
-  </si>
-  <si>
     <t>Contract Date</t>
   </si>
   <si>
@@ -362,13 +316,152 @@
   </si>
   <si>
     <t>This Excel file should provide details regarding the fields required for the data extract.  The format that this data is delivered in can either be a set of flat CSV files.  Each tab of this spreadsheet should describe the data expected in each file, section, or table and the diagram below has been provided to help navigate the relationships between the data in the tabs.  The diagram below uses standard crow's foot notation (see diagram on the right for assistance).</t>
+  </si>
+  <si>
+    <t>PrincipalAdvisorId</t>
+  </si>
+  <si>
+    <t>The user will be given employee-level access within the company</t>
+  </si>
+  <si>
+    <t>MGA Id</t>
+  </si>
+  <si>
+    <t>AGA Id</t>
+  </si>
+  <si>
+    <t>Carrier Id</t>
+  </si>
+  <si>
+    <t>*Cond</t>
+  </si>
+  <si>
+    <t>An existing AdvisorId within the organization</t>
+  </si>
+  <si>
+    <t>Advisor Id</t>
+  </si>
+  <si>
+    <t>An Identifier representing the advisor person  of this contract</t>
+  </si>
+  <si>
+    <t>There must be at least two parties entered per contract</t>
+  </si>
+  <si>
+    <t>An identifier representing the carrier of this contract if one exists</t>
+  </si>
+  <si>
+    <t>An identifier representing the MGA of this contract if one exists</t>
+  </si>
+  <si>
+    <t>An Identifier representing the AGA of this contract if one exists</t>
+  </si>
+  <si>
+    <t>An Identifier representing the first-level corporation of this contract if one exists</t>
+  </si>
+  <si>
+    <t>An Identifier representing the second-level corporation of this contract if one exists</t>
+  </si>
+  <si>
+    <t>MGA Internal Branch Id</t>
+  </si>
+  <si>
+    <t>Carrier Internal Branch Id</t>
+  </si>
+  <si>
+    <t>AGA Internal Branch Id</t>
+  </si>
+  <si>
+    <t>Corporation Id</t>
+  </si>
+  <si>
+    <t>Sub Corporation Id</t>
+  </si>
+  <si>
+    <t>An ID representing the Carrier branch with the contract if one exists.</t>
+  </si>
+  <si>
+    <t>An ID representing the MGA with the contract if one exists.</t>
+  </si>
+  <si>
+    <t>An ID representing the AGA with the contract if one exists.</t>
+  </si>
+  <si>
+    <t>Bulk Onboarding Id</t>
+  </si>
+  <si>
+    <t>An identifier that can be used to bulk onboard groups of companies.  This identifier is freeform and will be searchable in In-Trust.</t>
+  </si>
+  <si>
+    <t>An identifier that can be used to bulk onboard groups of advisors.  This identifier is freeform and will be searchable in In-Trust.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">APEXA is now supporting the contracting process at every level of the hierarchy, which means APEXA now needs details for every contract and corporation (as opposed to just the advisor and their corporation).  The primary changes are:
+1) Contract records for every party involved are now required.
+2) Full profile data is now required for every corporation and person involved in a contract.
+3) Full profile data is now required for one principal for every corporation and is linked to the corporate record.
+4) Advisor/corporation records now have an optional Group Onboarding Id that can be used in In-Trust to bulk onboard advisors/corporations.
+5) The format of the contract record has changed to better represent the data being requested (e.g. instead of a name and code for an MGA, an ID for a full profile must now be provided).
+Below is a conceptual diagram of the new contract table and how it relates to the advisor and company tables.  Once we receive data from all parties, we are expecting a contracting record that represents every permutation of the parties involved in a given contracting chain.  Each party is responsible for providing every permutation </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>they are involved in</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">.  In the diagram below there are 3 example contracts:
+1) Blue Contract: a direct contract from a carrier to an Advisor
+2) Green Contract: a direct contract from a carrier to a corporation, which has a sub-corporation, and is contracted to an advisor
+3) Red Contract: a carrier is contracted to a corporation via an MGA and an AGA, but has not contracted with an Advisor via that corporation yet
+In this example, Insurance Co (CA1226) must provide </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>at least</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the following records:
+CTR 1001 from Blue Contract
+CTR 1002, CTR1005, CTR1007 from Green Contract
+CTR 1008, CTR1010, CTR1013 from Red Contract
+Using the Red Contract as an example, our previous data specification would only have required CTR1013 from the carrier; however, since we now represent the full hierarchy of contracts, we now require CTR1008 (the carrier &amp; MGA contract) and CTR1010 (the carrier, MGA, and AGA contract) since these contracts facilitate CTR1013.  When the MGA in this scenario provides their data, we would require CTR1008, CTR1009, CTR1010, CTR1012, and CTR1013.</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -378,6 +471,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -405,7 +506,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -431,6 +532,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -455,6 +570,66 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>1846</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="5524500"/>
+          <a:ext cx="9612571" cy="8543925"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -815,104 +990,634 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet1"/>
-  <dimension ref="B2:W6"/>
+  <dimension ref="B2:Q39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.140625" customWidth="1"/>
+    <col min="17" max="17" width="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9"/>
-      <c r="S2" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="T2" s="10"/>
-      <c r="U2" s="10"/>
-      <c r="V2" s="10"/>
-      <c r="W2" s="10"/>
-    </row>
-    <row r="3" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
-      <c r="L3" s="9"/>
-      <c r="M3" s="9"/>
-      <c r="S3" s="10"/>
-      <c r="T3" s="10"/>
-      <c r="U3" s="10"/>
-      <c r="V3" s="10"/>
-      <c r="W3" s="10"/>
-    </row>
-    <row r="4" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
-      <c r="L4" s="9"/>
-      <c r="M4" s="9"/>
-    </row>
-    <row r="5" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="9"/>
-      <c r="L5" s="9"/>
-      <c r="M5" s="9"/>
-    </row>
-    <row r="6" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
-      <c r="K6" s="9"/>
-      <c r="L6" s="9"/>
-      <c r="M6" s="9"/>
+    <row r="2" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="15"/>
+      <c r="O2" s="15"/>
+      <c r="P2" s="15"/>
+      <c r="Q2" s="15"/>
+    </row>
+    <row r="3" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="15"/>
+      <c r="N3" s="15"/>
+      <c r="O3" s="15"/>
+      <c r="P3" s="15"/>
+      <c r="Q3" s="15"/>
+    </row>
+    <row r="4" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B4" s="15"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="15"/>
+      <c r="L4" s="15"/>
+      <c r="M4" s="15"/>
+      <c r="N4" s="15"/>
+      <c r="O4" s="15"/>
+      <c r="P4" s="15"/>
+      <c r="Q4" s="15"/>
+    </row>
+    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B5" s="15"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="15"/>
+      <c r="M5" s="15"/>
+      <c r="N5" s="15"/>
+      <c r="O5" s="15"/>
+      <c r="P5" s="15"/>
+      <c r="Q5" s="15"/>
+    </row>
+    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="15"/>
+      <c r="N6" s="15"/>
+      <c r="O6" s="15"/>
+      <c r="P6" s="15"/>
+      <c r="Q6" s="15"/>
+    </row>
+    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="15"/>
+      <c r="M7" s="15"/>
+      <c r="N7" s="15"/>
+      <c r="O7" s="15"/>
+      <c r="P7" s="15"/>
+      <c r="Q7" s="15"/>
+    </row>
+    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="15"/>
+      <c r="N8" s="15"/>
+      <c r="O8" s="15"/>
+      <c r="P8" s="15"/>
+      <c r="Q8" s="15"/>
+    </row>
+    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="15"/>
+      <c r="M9" s="15"/>
+      <c r="N9" s="15"/>
+      <c r="O9" s="15"/>
+      <c r="P9" s="15"/>
+      <c r="Q9" s="15"/>
+    </row>
+    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="15"/>
+      <c r="L10" s="15"/>
+      <c r="M10" s="15"/>
+      <c r="N10" s="15"/>
+      <c r="O10" s="15"/>
+      <c r="P10" s="15"/>
+      <c r="Q10" s="15"/>
+    </row>
+    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B11" s="15"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
+      <c r="L11" s="15"/>
+      <c r="M11" s="15"/>
+      <c r="N11" s="15"/>
+      <c r="O11" s="15"/>
+      <c r="P11" s="15"/>
+      <c r="Q11" s="15"/>
+    </row>
+    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="15"/>
+      <c r="L12" s="15"/>
+      <c r="M12" s="15"/>
+      <c r="N12" s="15"/>
+      <c r="O12" s="15"/>
+      <c r="P12" s="15"/>
+      <c r="Q12" s="15"/>
+    </row>
+    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="15"/>
+      <c r="M13" s="15"/>
+      <c r="N13" s="15"/>
+      <c r="O13" s="15"/>
+      <c r="P13" s="15"/>
+      <c r="Q13" s="15"/>
+    </row>
+    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="15"/>
+      <c r="J14" s="15"/>
+      <c r="K14" s="15"/>
+      <c r="L14" s="15"/>
+      <c r="M14" s="15"/>
+      <c r="N14" s="15"/>
+      <c r="O14" s="15"/>
+      <c r="P14" s="15"/>
+      <c r="Q14" s="15"/>
+    </row>
+    <row r="15" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B15" s="15"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="15"/>
+      <c r="K15" s="15"/>
+      <c r="L15" s="15"/>
+      <c r="M15" s="15"/>
+      <c r="N15" s="15"/>
+      <c r="O15" s="15"/>
+      <c r="P15" s="15"/>
+      <c r="Q15" s="15"/>
+    </row>
+    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B16" s="15"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="15"/>
+      <c r="J16" s="15"/>
+      <c r="K16" s="15"/>
+      <c r="L16" s="15"/>
+      <c r="M16" s="15"/>
+      <c r="N16" s="15"/>
+      <c r="O16" s="15"/>
+      <c r="P16" s="15"/>
+      <c r="Q16" s="15"/>
+    </row>
+    <row r="17" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B17" s="15"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="15"/>
+      <c r="K17" s="15"/>
+      <c r="L17" s="15"/>
+      <c r="M17" s="15"/>
+      <c r="N17" s="15"/>
+      <c r="O17" s="15"/>
+      <c r="P17" s="15"/>
+      <c r="Q17" s="15"/>
+    </row>
+    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B18" s="15"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
+      <c r="I18" s="15"/>
+      <c r="J18" s="15"/>
+      <c r="K18" s="15"/>
+      <c r="L18" s="15"/>
+      <c r="M18" s="15"/>
+      <c r="N18" s="15"/>
+      <c r="O18" s="15"/>
+      <c r="P18" s="15"/>
+      <c r="Q18" s="15"/>
+    </row>
+    <row r="19" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B19" s="15"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
+      <c r="I19" s="15"/>
+      <c r="J19" s="15"/>
+      <c r="K19" s="15"/>
+      <c r="L19" s="15"/>
+      <c r="M19" s="15"/>
+      <c r="N19" s="15"/>
+      <c r="O19" s="15"/>
+      <c r="P19" s="15"/>
+      <c r="Q19" s="15"/>
+    </row>
+    <row r="20" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B20" s="15"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15"/>
+      <c r="I20" s="15"/>
+      <c r="J20" s="15"/>
+      <c r="K20" s="15"/>
+      <c r="L20" s="15"/>
+      <c r="M20" s="15"/>
+      <c r="N20" s="15"/>
+      <c r="O20" s="15"/>
+      <c r="P20" s="15"/>
+      <c r="Q20" s="15"/>
+    </row>
+    <row r="21" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B21" s="15"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="15"/>
+      <c r="I21" s="15"/>
+      <c r="J21" s="15"/>
+      <c r="K21" s="15"/>
+      <c r="L21" s="15"/>
+      <c r="M21" s="15"/>
+      <c r="N21" s="15"/>
+      <c r="O21" s="15"/>
+      <c r="P21" s="15"/>
+      <c r="Q21" s="15"/>
+    </row>
+    <row r="22" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B22" s="15"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="15"/>
+      <c r="I22" s="15"/>
+      <c r="J22" s="15"/>
+      <c r="K22" s="15"/>
+      <c r="L22" s="15"/>
+      <c r="M22" s="15"/>
+      <c r="N22" s="15"/>
+      <c r="O22" s="15"/>
+      <c r="P22" s="15"/>
+      <c r="Q22" s="15"/>
+    </row>
+    <row r="23" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B23" s="15"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="15"/>
+      <c r="I23" s="15"/>
+      <c r="J23" s="15"/>
+      <c r="K23" s="15"/>
+      <c r="L23" s="15"/>
+      <c r="M23" s="15"/>
+      <c r="N23" s="15"/>
+      <c r="O23" s="15"/>
+      <c r="P23" s="15"/>
+      <c r="Q23" s="15"/>
+    </row>
+    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B24" s="15"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="15"/>
+      <c r="H24" s="15"/>
+      <c r="I24" s="15"/>
+      <c r="J24" s="15"/>
+      <c r="K24" s="15"/>
+      <c r="L24" s="15"/>
+      <c r="M24" s="15"/>
+      <c r="N24" s="15"/>
+      <c r="O24" s="15"/>
+      <c r="P24" s="15"/>
+      <c r="Q24" s="15"/>
+    </row>
+    <row r="25" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B25" s="15"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="15"/>
+      <c r="H25" s="15"/>
+      <c r="I25" s="15"/>
+      <c r="J25" s="15"/>
+      <c r="K25" s="15"/>
+      <c r="L25" s="15"/>
+      <c r="M25" s="15"/>
+      <c r="N25" s="15"/>
+      <c r="O25" s="15"/>
+      <c r="P25" s="15"/>
+      <c r="Q25" s="15"/>
+    </row>
+    <row r="26" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B26" s="15"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="15"/>
+      <c r="G26" s="15"/>
+      <c r="H26" s="15"/>
+      <c r="I26" s="15"/>
+      <c r="J26" s="15"/>
+      <c r="K26" s="15"/>
+      <c r="L26" s="15"/>
+      <c r="M26" s="15"/>
+      <c r="N26" s="15"/>
+      <c r="O26" s="15"/>
+      <c r="P26" s="15"/>
+      <c r="Q26" s="15"/>
+    </row>
+    <row r="27" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B27" s="15"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="15"/>
+      <c r="H27" s="15"/>
+      <c r="I27" s="15"/>
+      <c r="J27" s="15"/>
+      <c r="K27" s="15"/>
+      <c r="L27" s="15"/>
+      <c r="M27" s="15"/>
+      <c r="N27" s="15"/>
+      <c r="O27" s="15"/>
+      <c r="P27" s="15"/>
+      <c r="Q27" s="15"/>
+    </row>
+    <row r="28" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B28" s="15"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="15"/>
+      <c r="F28" s="15"/>
+      <c r="G28" s="15"/>
+      <c r="H28" s="15"/>
+      <c r="I28" s="15"/>
+      <c r="J28" s="15"/>
+      <c r="K28" s="15"/>
+      <c r="L28" s="15"/>
+      <c r="M28" s="15"/>
+      <c r="N28" s="15"/>
+      <c r="O28" s="15"/>
+      <c r="P28" s="15"/>
+      <c r="Q28" s="15"/>
+    </row>
+    <row r="29" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="15"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="15"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="15"/>
+      <c r="G29" s="15"/>
+      <c r="H29" s="15"/>
+      <c r="I29" s="15"/>
+      <c r="J29" s="15"/>
+      <c r="K29" s="15"/>
+      <c r="L29" s="15"/>
+      <c r="M29" s="15"/>
+      <c r="N29" s="15"/>
+      <c r="O29" s="15"/>
+      <c r="P29" s="15"/>
+      <c r="Q29" s="15"/>
+    </row>
+    <row r="30" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I30" s="9"/>
+      <c r="J30" s="9"/>
+      <c r="K30" s="9"/>
+      <c r="L30" s="9"/>
+      <c r="M30" s="9"/>
+      <c r="N30" s="9"/>
+      <c r="O30" s="9"/>
+      <c r="P30" s="9"/>
+      <c r="Q30" s="9"/>
+    </row>
+    <row r="31" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I31" s="9"/>
+      <c r="J31" s="9"/>
+      <c r="K31" s="9"/>
+      <c r="L31" s="9"/>
+      <c r="M31" s="9"/>
+      <c r="N31" s="9"/>
+      <c r="O31" s="9"/>
+      <c r="P31" s="9"/>
+      <c r="Q31" s="9"/>
+    </row>
+    <row r="32" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I32" s="9"/>
+      <c r="J32" s="9"/>
+      <c r="K32" s="9"/>
+      <c r="L32" s="9"/>
+      <c r="M32" s="9"/>
+      <c r="N32" s="9"/>
+      <c r="O32" s="9"/>
+      <c r="P32" s="9"/>
+      <c r="Q32" s="9"/>
+    </row>
+    <row r="33" spans="9:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I33" s="9"/>
+      <c r="J33" s="9"/>
+      <c r="K33" s="9"/>
+      <c r="L33" s="9"/>
+      <c r="M33" s="9"/>
+      <c r="N33" s="9"/>
+      <c r="O33" s="9"/>
+      <c r="P33" s="9"/>
+      <c r="Q33" s="9"/>
+    </row>
+    <row r="34" spans="9:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I34" s="9"/>
+      <c r="J34" s="9"/>
+      <c r="K34" s="9"/>
+      <c r="L34" s="9"/>
+      <c r="M34" s="9"/>
+      <c r="N34" s="9"/>
+      <c r="O34" s="9"/>
+      <c r="P34" s="9"/>
+      <c r="Q34" s="9"/>
+    </row>
+    <row r="35" spans="9:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I35" s="9"/>
+      <c r="J35" s="9"/>
+      <c r="K35" s="9"/>
+      <c r="L35" s="9"/>
+      <c r="M35" s="9"/>
+      <c r="N35" s="9"/>
+      <c r="O35" s="9"/>
+      <c r="P35" s="9"/>
+      <c r="Q35" s="9"/>
+    </row>
+    <row r="36" spans="9:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I36" s="9"/>
+      <c r="J36" s="9"/>
+      <c r="K36" s="9"/>
+      <c r="L36" s="9"/>
+      <c r="M36" s="9"/>
+      <c r="N36" s="9"/>
+      <c r="O36" s="9"/>
+      <c r="P36" s="9"/>
+      <c r="Q36" s="9"/>
+    </row>
+    <row r="37" spans="9:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I37" s="9"/>
+      <c r="J37" s="9"/>
+      <c r="K37" s="9"/>
+      <c r="L37" s="9"/>
+      <c r="M37" s="9"/>
+      <c r="N37" s="9"/>
+      <c r="O37" s="9"/>
+      <c r="P37" s="9"/>
+      <c r="Q37" s="9"/>
+    </row>
+    <row r="38" spans="9:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I38" s="9"/>
+      <c r="J38" s="9"/>
+      <c r="K38" s="9"/>
+      <c r="L38" s="9"/>
+      <c r="M38" s="9"/>
+      <c r="N38" s="9"/>
+      <c r="O38" s="9"/>
+      <c r="P38" s="9"/>
+      <c r="Q38" s="9"/>
+    </row>
+    <row r="39" spans="9:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I39" s="9"/>
+      <c r="J39" s="9"/>
+      <c r="K39" s="9"/>
+      <c r="L39" s="9"/>
+      <c r="M39" s="9"/>
+      <c r="N39" s="9"/>
+      <c r="O39" s="9"/>
+      <c r="P39" s="9"/>
+      <c r="Q39" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B2:M6"/>
-    <mergeCell ref="S2:W3"/>
+  <mergeCells count="1">
+    <mergeCell ref="B2:Q29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -920,10 +1625,10 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:E14"/>
+  <sheetPr codeName="Sheet9"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -953,53 +1658,53 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>46</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>13</v>
-      </c>
       <c r="D2" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>16</v>
+        <v>47</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>32</v>
-      </c>
+      <c r="C4" s="7"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>13</v>
-      </c>
+      <c r="A5" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>4</v>
+        <v>73</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>32</v>
@@ -1007,87 +1712,19 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" s="7"/>
-      <c r="D14" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="E14" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1095,10 +1732,119 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="B2:W6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q5" sqref="Q5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="9.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
+      <c r="S2" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="T2" s="16"/>
+      <c r="U2" s="16"/>
+      <c r="V2" s="16"/>
+      <c r="W2" s="16"/>
+    </row>
+    <row r="3" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="15"/>
+      <c r="S3" s="16"/>
+      <c r="T3" s="16"/>
+      <c r="U3" s="16"/>
+      <c r="V3" s="16"/>
+      <c r="W3" s="16"/>
+    </row>
+    <row r="4" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B4" s="15"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="15"/>
+      <c r="L4" s="15"/>
+      <c r="M4" s="15"/>
+    </row>
+    <row r="5" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B5" s="15"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="15"/>
+      <c r="M5" s="15"/>
+    </row>
+    <row r="6" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="15"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:M6"/>
+    <mergeCell ref="S2:W3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:E9"/>
+  <sheetPr codeName="Sheet2"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1130,7 +1876,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>12</v>
@@ -1139,56 +1885,50 @@
         <v>13</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B5" s="3">
-        <v>999999999</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B6" s="3">
-        <v>9999999999</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>87</v>
+        <v>4</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>32</v>
@@ -1199,24 +1939,87 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>57</v>
+        <v>19</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="B9" s="7" t="s">
+      <c r="A9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="E9" s="8"/>
+      <c r="C10" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="7"/>
+      <c r="D14" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="E14" s="8"/>
+    </row>
+    <row r="15" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>121</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1225,6 +2028,164 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet3"/>
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="11" style="3" customWidth="1"/>
+    <col min="4" max="4" width="44.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="32.5703125" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="3">
+        <v>999999999</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="3">
+        <v>9999999999</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="7"/>
+      <c r="D10" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="E10" s="8"/>
+    </row>
+    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="12"/>
+      <c r="D11" s="11" t="s">
+        <v>120</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:E10"/>
@@ -1299,7 +2260,7 @@
         <v>45</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1374,7 +2335,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:E7"/>
@@ -1449,7 +2410,7 @@
         <v>51</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1483,252 +2444,6 @@
       </c>
       <c r="D7" s="2" t="s">
         <v>59</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet6"/>
-  <dimension ref="A1:E16"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="28.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="21.42578125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="11" style="3" customWidth="1"/>
-    <col min="4" max="4" width="44.7109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="32.5703125" style="2" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="E6" s="8"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="E7" s="8"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -1738,6 +2453,281 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet6"/>
+  <dimension ref="A1:E24"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20:E26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="49.5703125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="32.5703125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="53.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="7"/>
+      <c r="D3" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="E4" s="11"/>
+    </row>
+    <row r="5" spans="1:5" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="D5" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="E5" s="11"/>
+    </row>
+    <row r="6" spans="1:5" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="E6" s="11"/>
+    </row>
+    <row r="7" spans="1:5" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="7"/>
+      <c r="D7" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="E7" s="11"/>
+    </row>
+    <row r="8" spans="1:5" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="E8" s="11"/>
+    </row>
+    <row r="9" spans="1:5" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="7"/>
+      <c r="D9" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="E9" s="11"/>
+    </row>
+    <row r="10" spans="1:5" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="E10" s="11"/>
+    </row>
+    <row r="11" spans="1:5" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="E11" s="11"/>
+    </row>
+    <row r="12" spans="1:5" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="E12" s="11"/>
+    </row>
+    <row r="13" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C18" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="9"/>
+      <c r="B20" s="9"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="10"/>
+      <c r="B24" s="12"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:E4"/>
@@ -1781,7 +2771,7 @@
         <v>13</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -1795,18 +2785,18 @@
         <v>13</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>32</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -1815,7 +2805,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:E12"/>
@@ -1919,12 +2909,12 @@
         <v>32</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>31</v>
@@ -1954,120 +2944,13 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>32</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>13</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet9"/>
-  <dimension ref="A1:E8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="28.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="21.42578125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="11" style="3" customWidth="1"/>
-    <col min="4" max="4" width="44.7109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="32.5703125" style="2" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Correct Bulk Onboarding Id field name in changelog.
</commit_message>
<xml_diff>
--- a/InTrust-FileFormatSpecification.xlsx
+++ b/InTrust-FileFormatSpecification.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="V:\Drive\BlueSun\APEXA\System Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="V:\Source\GIT\intrust-file-specification\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -401,7 +401,7 @@
 1) Contract records for every party involved are now required.
 2) Full profile data is now required for every corporation and person involved in a contract.
 3) Full profile data is now required for one principal for every corporation and is linked to the corporate record.
-4) Advisor/corporation records now have an optional Group Onboarding Id that can be used in In-Trust to bulk onboard advisors/corporations.
+4) Advisor/corporation records now have an optional Bulk Onboarding Id that can be used in In-Trust to bulk onboard advisors/corporations.
 5) The format of the contract record has changed to better represent the data being requested (e.g. instead of a name and code for an MGA, an ID for a full profile must now be provided).
 Below is a conceptual diagram of the new contract table and how it relates to the advisor and company tables.  Once we receive data from all parties, we are expecting a contracting record that represents every permutation of the parties involved in a given contracting chain.  Each party is responsible for providing every permutation </t>
     </r>

</xml_diff>

<commit_message>
update intrust file spec
</commit_message>
<xml_diff>
--- a/InTrust-FileFormatSpecification.xlsx
+++ b/InTrust-FileFormatSpecification.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17927"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kelsi.elshaw\Desktop\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="744" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12360" tabRatio="744" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Data Diagram" sheetId="8" r:id="rId1"/>
@@ -200,14 +205,160 @@
     <t>An identifier that can be used to bulk onboard groups of advisors.  This identifier is freeform and will be searchable in In-Trust.</t>
   </si>
   <si>
+    <t>Internal Branch Id</t>
+  </si>
+  <si>
+    <t>Internal Branch Name</t>
+  </si>
+  <si>
+    <t>MGA Branch Code</t>
+  </si>
+  <si>
+    <t>MGA Code</t>
+  </si>
+  <si>
+    <t>AGA Branch Code</t>
+  </si>
+  <si>
+    <t>AGA Code</t>
+  </si>
+  <si>
+    <t>Corporation Code</t>
+  </si>
+  <si>
+    <t>Carrier-issued MGA selling code</t>
+  </si>
+  <si>
+    <t>Carrier-issued AGA selling code</t>
+  </si>
+  <si>
+    <t>Carrier-issued Corporation selling code</t>
+  </si>
+  <si>
+    <t>True/False</t>
+  </si>
+  <si>
+    <t>Days Before Termination Notice</t>
+  </si>
+  <si>
+    <t>Minimum Coverage Required</t>
+  </si>
+  <si>
+    <t>Require Shareholder Signature</t>
+  </si>
+  <si>
+    <t>Collect SIN</t>
+  </si>
+  <si>
+    <t>Useable By Third Party</t>
+  </si>
+  <si>
+    <t>Retention Period</t>
+  </si>
+  <si>
+    <t>Minimum coverage required in dollar amount</t>
+  </si>
+  <si>
+    <t>Requires Prior Business</t>
+  </si>
+  <si>
+    <t>Payment Options</t>
+  </si>
+  <si>
+    <t>Banking Required</t>
+  </si>
+  <si>
+    <t>Direct Deposit Only</t>
+  </si>
+  <si>
+    <t>Cheque By Mail Only</t>
+  </si>
+  <si>
+    <t>Both</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Minimum number days of notice to be provided before terminating a contract</t>
+  </si>
+  <si>
+    <t>Requires advisor to have business prior to contracting</t>
+  </si>
+  <si>
+    <t>Contract requires a copy of all shareholder signatures to be uploaded</t>
+  </si>
+  <si>
+    <t>Collect SIN from the implicated advisor</t>
+  </si>
+  <si>
+    <t>Indicates if the contracting package can be used by third parties</t>
+  </si>
+  <si>
+    <t>Number of years the documents associated with a contract are kept in the system after termination</t>
+  </si>
+  <si>
+    <t>The name of the branch.</t>
+  </si>
+  <si>
+    <t>Carrier-issued MGA branch code</t>
+  </si>
+  <si>
+    <t>Carrier-issued AGA branch code</t>
+  </si>
+  <si>
+    <t>Defaulted to English</t>
+  </si>
+  <si>
+    <t>Needed for attestation and deduplication.</t>
+  </si>
+  <si>
+    <t>The immediate branch that the advisor reports to, internal to your organization.</t>
+  </si>
+  <si>
+    <t>Defaulted to $0</t>
+  </si>
+  <si>
+    <t>Defaulted to 30</t>
+  </si>
+  <si>
+    <t>Defaulted to False</t>
+  </si>
+  <si>
+    <t>Defaulted to Both</t>
+  </si>
+  <si>
+    <t>Defaulted to 7</t>
+  </si>
+  <si>
+    <t>Defaulted to True</t>
+  </si>
+  <si>
+    <t>Overridden by Payment Options</t>
+  </si>
+  <si>
+    <t>English/French</t>
+  </si>
+  <si>
+    <t>Active/Vested</t>
+  </si>
+  <si>
+    <t>** Accepted Values</t>
+  </si>
+  <si>
+    <t>**Text</t>
+  </si>
+  <si>
+    <t>See below for accepted values</t>
+  </si>
+  <si>
     <r>
-      <t xml:space="preserve">APEXA is now supporting the contracting process at every level of the hierarchy, which means APEXA now needs details for every contract and corporation (as opposed to just the advisor and their corporation).  The primary changes are:
-1) Contract records for every party involved are now required.
-2) Full profile data is now required for every corporation and person involved in a contract.
-3) Full profile data is now required for one principal for every corporation and is linked to the corporate record.
-4) Advisor/corporation records now have an optional Bulk Onboarding Id that can be used in In-Trust to bulk onboard advisors/corporations.
-5) The format of the contract record has changed to better represent the data being requested (e.g. instead of a name and code for an MGA, an ID for a full profile must now be provided).
-Below is a conceptual diagram of the new contract table and how it relates to the advisor and company tables.  Once we receive data from all parties, we are expecting a contracting record that represents every permutation of the parties involved in a given contracting chain.  Each party is responsible for providing every permutation </t>
+      <t xml:space="preserve">APEXA supports the contracting process at every level of the hierarchy, which means APEXA needs the following details for every contract and corporation:
+1) Contract records for every party involved are required.
+2) Full profile data is required for every corporation and person involved in a contract.
+3) Full profile data is required for one principal for every corporation and is linked to the corporate record.
+4) Advisor/corporation records have an optional Bulk Onboarding Id that can be used in In-Trust to bulk onboard advisors/corporations.
+Below is a conceptual diagram of the contract table and how it relates to the advisor and company tables.  Once we receive data from all parties, we are expecting a contracting record that represents every permutation of the parties involved in a given contracting chain.  Each party is responsible for providing every permutation </t>
     </r>
     <r>
       <rPr>
@@ -257,161 +408,14 @@
 CTR 1001 from Blue Contract
 CTR 1002, CTR1005, CTR1007 from Green Contract
 CTR 1008, CTR1010, CTR1013 from Red Contract
-Using the Red Contract as an example, our previous data specification would only have required CTR1013 from the carrier; however, since we now represent the full hierarchy of contracts, we now require CTR1008 (the carrier &amp; MGA contract) and CTR1010 (the carrier, MGA, and AGA contract) since these contracts facilitate CTR1013.  When the MGA in this scenario provides their data, we would require CTR1008, CTR1009, CTR1010, CTR1012, and CTR1013.</t>
+Using the Red Contract as an example, we require CTR1008 (the carrier &amp; MGA contract) and CTR1010 (the carrier, MGA, and AGA contract) since these contracts facilitate CTR1013.  When the MGA in this scenario provides their data, we would require CTR1008, CTR1009, CTR1010, CTR1012, and CTR1013.</t>
     </r>
-  </si>
-  <si>
-    <t>Internal Branch Id</t>
-  </si>
-  <si>
-    <t>Internal Branch Name</t>
-  </si>
-  <si>
-    <t>MGA Branch Code</t>
-  </si>
-  <si>
-    <t>MGA Code</t>
-  </si>
-  <si>
-    <t>AGA Branch Code</t>
-  </si>
-  <si>
-    <t>AGA Code</t>
-  </si>
-  <si>
-    <t>Corporation Code</t>
-  </si>
-  <si>
-    <t>Carrier-issued MGA selling code</t>
-  </si>
-  <si>
-    <t>Carrier-issued AGA selling code</t>
-  </si>
-  <si>
-    <t>Carrier-issued Corporation selling code</t>
-  </si>
-  <si>
-    <t>True/False</t>
-  </si>
-  <si>
-    <t>Days Before Termination Notice</t>
-  </si>
-  <si>
-    <t>Minimum Coverage Required</t>
-  </si>
-  <si>
-    <t>Require Shareholder Signature</t>
-  </si>
-  <si>
-    <t>Collect SIN</t>
-  </si>
-  <si>
-    <t>Useable By Third Party</t>
-  </si>
-  <si>
-    <t>Retention Period</t>
-  </si>
-  <si>
-    <t>Minimum coverage required in dollar amount</t>
-  </si>
-  <si>
-    <t>Requires Prior Business</t>
-  </si>
-  <si>
-    <t>Payment Options</t>
-  </si>
-  <si>
-    <t>Banking Required</t>
-  </si>
-  <si>
-    <t>Direct Deposit Only</t>
-  </si>
-  <si>
-    <t>Cheque By Mail Only</t>
-  </si>
-  <si>
-    <t>Both</t>
-  </si>
-  <si>
-    <t>None</t>
-  </si>
-  <si>
-    <t>Minimum number days of notice to be provided before terminating a contract</t>
-  </si>
-  <si>
-    <t>Requires advisor to have business prior to contracting</t>
-  </si>
-  <si>
-    <t>Contract requires a copy of all shareholder signatures to be uploaded</t>
-  </si>
-  <si>
-    <t>Collect SIN from the implicated advisor</t>
-  </si>
-  <si>
-    <t>Indicates if the contracting package can be used by third parties</t>
-  </si>
-  <si>
-    <t>Number of years the documents associated with a contract are kept in the system after termination</t>
-  </si>
-  <si>
-    <t>The name of the branch.</t>
-  </si>
-  <si>
-    <t>Carrier-issued MGA branch code</t>
-  </si>
-  <si>
-    <t>Carrier-issued AGA branch code</t>
-  </si>
-  <si>
-    <t>Defaulted to English</t>
-  </si>
-  <si>
-    <t>Needed for attestation and deduplication.</t>
-  </si>
-  <si>
-    <t>The immediate branch that the advisor reports to, internal to your organization.</t>
-  </si>
-  <si>
-    <t>Defaulted to $0</t>
-  </si>
-  <si>
-    <t>Defaulted to 30</t>
-  </si>
-  <si>
-    <t>Defaulted to False</t>
-  </si>
-  <si>
-    <t>Defaulted to Both</t>
-  </si>
-  <si>
-    <t>Defaulted to 7</t>
-  </si>
-  <si>
-    <t>Defaulted to True</t>
-  </si>
-  <si>
-    <t>Overridden by Payment Options</t>
-  </si>
-  <si>
-    <t>English/French</t>
-  </si>
-  <si>
-    <t>Active/Vested</t>
-  </si>
-  <si>
-    <t>** Accepted Values</t>
-  </si>
-  <si>
-    <t>**Text</t>
-  </si>
-  <si>
-    <t>See below for accepted values</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -599,7 +603,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" descr="http://3.bp.blogspot.com/-4t71515irAM/ToVZHu4yF-I/AAAAAAAAALY/AJFTZ8FA2AY/s1600/crowsfoot_notation.gif"/>
+        <xdr:cNvPr id="2" name="Picture 1" descr="http://3.bp.blogspot.com/-4t71515irAM/ToVZHu4yF-I/AAAAAAAAALY/AJFTZ8FA2AY/s1600/crowsfoot_notation.gif">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -654,7 +664,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Picture 5"/>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -714,7 +730,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1012,7 +1034,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1216,8 +1238,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:Q39"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="W23" sqref="W23"/>
+    <sheetView topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="U84" sqref="U84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1227,7 +1249,7 @@
   <sheetData>
     <row r="2" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="24" t="s">
-        <v>60</v>
+        <v>109</v>
       </c>
       <c r="C2" s="24"/>
       <c r="D2" s="24"/>
@@ -1856,8 +1878,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1965,11 +1987,11 @@
         <v>17</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D9" s="11"/>
       <c r="E9" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -2009,26 +2031,26 @@
     </row>
     <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B13" s="12" t="s">
         <v>9</v>
       </c>
       <c r="C13" s="9"/>
       <c r="D13" s="17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B14" s="12" t="s">
         <v>9</v>
       </c>
       <c r="C14" s="9"/>
       <c r="D14" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -2044,7 +2066,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2117,7 +2139,7 @@
         <v>999999999</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2128,7 +2150,7 @@
         <v>9999999999</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -2147,12 +2169,12 @@
         <v>17</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C8" s="12"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -2201,8 +2223,8 @@
   </sheetPr>
   <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2279,27 +2301,27 @@
     </row>
     <row r="5" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B5" s="23" t="s">
         <v>9</v>
       </c>
       <c r="C5" s="23"/>
       <c r="D5" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E5" s="17"/>
     </row>
     <row r="6" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B6" s="23" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="23"/>
       <c r="D6" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E6" s="17"/>
     </row>
@@ -2320,27 +2342,27 @@
     </row>
     <row r="8" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B8" s="23" t="s">
         <v>9</v>
       </c>
       <c r="C8" s="23"/>
       <c r="D8" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E8" s="17"/>
     </row>
     <row r="9" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B9" s="23" t="s">
         <v>9</v>
       </c>
       <c r="C9" s="23"/>
       <c r="D9" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E9" s="17"/>
     </row>
@@ -2361,14 +2383,14 @@
     </row>
     <row r="11" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B11" s="23" t="s">
         <v>9</v>
       </c>
       <c r="C11" s="23"/>
       <c r="D11" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E11" s="17"/>
     </row>
@@ -2422,7 +2444,7 @@
         <v>31</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C15" s="16"/>
       <c r="D15" s="9"/>
@@ -2462,137 +2484,137 @@
     </row>
     <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B18" s="23" t="s">
         <v>0</v>
       </c>
       <c r="C18" s="23"/>
       <c r="D18" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B19" s="23" t="s">
         <v>0</v>
       </c>
       <c r="C19" s="23"/>
       <c r="D19" s="17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B20" s="23" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C20" s="23"/>
       <c r="D20" s="17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E20" s="17" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B21" s="23" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C21" s="23"/>
       <c r="D21" s="17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E21" s="17" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B22" s="23" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C22" s="23"/>
       <c r="D22" s="17" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B23" s="23" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C23" s="23"/>
       <c r="D23" s="17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B24" s="23" t="s">
         <v>0</v>
       </c>
       <c r="C24" s="23"/>
       <c r="D24" s="17" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B25" s="23" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C25" s="23"/>
       <c r="D25" s="17" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B26" s="23" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C26" s="23"/>
       <c r="D26" s="17" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2620,27 +2642,27 @@
     </row>
     <row r="30" spans="1:5" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D30" s="15" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="D31" s="13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D32" s="13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="33" spans="4:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D33" s="13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="34" spans="4:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D34" s="14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="35" spans="4:4" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>

</xml_diff>